<commit_message>
add combined IQ to mixed models
</commit_message>
<xml_diff>
--- a/220222_all_neuropsych.xlsx
+++ b/220222_all_neuropsych.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evsnyder/Documents/MH/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{28391736-254A-464A-8842-99C923096539}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{25816EF9-9775-C448-8DD6-3728944469F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10200" yWindow="4800" windowWidth="31820" windowHeight="21220"/>
+    <workbookView xWindow="12780" yWindow="6900" windowWidth="26840" windowHeight="15940"/>
   </bookViews>
   <sheets>
     <sheet name="DirectBrainRecording-Demographi" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2701" uniqueCount="754">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2694" uniqueCount="748">
   <si>
     <t>Subject Number</t>
   </si>
@@ -2065,12 +2065,6 @@
     <t>R1552E-Neuropsychologic Report-retracted.pdf</t>
   </si>
   <si>
-    <t>33/63</t>
-  </si>
-  <si>
-    <t>20/63</t>
-  </si>
-  <si>
     <t>R1553E-Neuropsychologic Report-retracted.pdf</t>
   </si>
   <si>
@@ -2104,9 +2098,6 @@
     <t>was hit by a car when  was nine.  put a dent in the hood and had to learn to walk and talk again; recovered in a couple of weeks, occurred in 1989, had to wear a foot ball helmet. Fell often later in life related to drug use</t>
   </si>
   <si>
-    <t>34/63</t>
-  </si>
-  <si>
     <t>R1561E-Neuropsychologic Report_redacted.pdf</t>
   </si>
   <si>
@@ -2134,9 +2125,6 @@
     <t xml:space="preserve">Head Trauma with LOC: Yes, in 2017 MVI w/head trauma, R frontal craniotomy </t>
   </si>
   <si>
-    <t>18/63</t>
-  </si>
-  <si>
     <t>R1568E-Neuropsychologic Report_redacted.pdf</t>
   </si>
   <si>
@@ -2194,16 +2182,10 @@
     <t>R1580D_Neuropsych_15Feb2021.pdf</t>
   </si>
   <si>
-    <t>14/63</t>
-  </si>
-  <si>
     <t>R1581E-Neuropsychologic Report_redacted.pdf</t>
   </si>
   <si>
     <t>RNS implant (Neuropace)</t>
-  </si>
-  <si>
-    <t>23/63</t>
   </si>
   <si>
     <t>R1582E-Neuropsychologic Report_redacted.pdf</t>
@@ -2765,10 +2747,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3126,9 +3107,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z601"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -24234,11 +24213,11 @@
       <c r="I554" s="1">
         <v>44302</v>
       </c>
-      <c r="L554" t="s">
-        <v>681</v>
-      </c>
-      <c r="M554" t="s">
-        <v>682</v>
+      <c r="L554">
+        <v>33</v>
+      </c>
+      <c r="M554">
+        <v>20</v>
       </c>
       <c r="R554">
         <v>89</v>
@@ -24247,7 +24226,7 @@
         <v>75</v>
       </c>
       <c r="V554" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
     </row>
     <row r="555" spans="1:24" x14ac:dyDescent="0.2">
@@ -24273,7 +24252,7 @@
         <v>44298</v>
       </c>
       <c r="J555" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="P555">
         <v>98</v>
@@ -24288,7 +24267,7 @@
         <v>7</v>
       </c>
       <c r="V555" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
     <row r="556" spans="1:24" x14ac:dyDescent="0.2">
@@ -24335,7 +24314,7 @@
         <v>105</v>
       </c>
       <c r="V556" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="557" spans="1:24" x14ac:dyDescent="0.2">
@@ -24379,13 +24358,13 @@
         <v>102</v>
       </c>
       <c r="V557" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="W557" t="s">
         <v>49</v>
       </c>
       <c r="X557" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
     </row>
     <row r="558" spans="1:24" x14ac:dyDescent="0.2">
@@ -24446,7 +24425,7 @@
         <v>5</v>
       </c>
       <c r="V559" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="W559" t="s">
         <v>101</v>
@@ -24496,7 +24475,7 @@
         <v>82</v>
       </c>
       <c r="V560" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
     </row>
     <row r="561" spans="1:24" x14ac:dyDescent="0.2">
@@ -24522,7 +24501,7 @@
         <v>44341</v>
       </c>
       <c r="J561" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="P561">
         <v>87</v>
@@ -24537,7 +24516,7 @@
         <v>8</v>
       </c>
       <c r="V561" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
     </row>
     <row r="562" spans="1:24" x14ac:dyDescent="0.2">
@@ -24566,13 +24545,13 @@
         <v>44342</v>
       </c>
       <c r="J562" t="s">
-        <v>693</v>
-      </c>
-      <c r="L562" t="s">
-        <v>682</v>
-      </c>
-      <c r="M562" t="s">
-        <v>694</v>
+        <v>691</v>
+      </c>
+      <c r="L562">
+        <v>20</v>
+      </c>
+      <c r="M562">
+        <v>34</v>
       </c>
       <c r="Q562">
         <v>95</v>
@@ -24584,7 +24563,7 @@
         <v>98</v>
       </c>
       <c r="V562" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
     </row>
     <row r="563" spans="1:24" x14ac:dyDescent="0.2">
@@ -24633,7 +24612,7 @@
         <v>44355</v>
       </c>
       <c r="J564" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="P564">
         <v>78</v>
@@ -24648,7 +24627,7 @@
         <v>6</v>
       </c>
       <c r="V564" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="W564" t="s">
         <v>58</v>
@@ -24698,13 +24677,13 @@
         <v>100</v>
       </c>
       <c r="V565" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
       <c r="W565" t="s">
         <v>49</v>
       </c>
       <c r="X565" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
     </row>
     <row r="566" spans="1:24" x14ac:dyDescent="0.2">
@@ -24745,7 +24724,7 @@
         <v>8</v>
       </c>
       <c r="V566" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
     </row>
     <row r="567" spans="1:24" x14ac:dyDescent="0.2">
@@ -24792,7 +24771,7 @@
         <v>77</v>
       </c>
       <c r="V567" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
     </row>
     <row r="568" spans="1:24" x14ac:dyDescent="0.2">
@@ -24830,7 +24809,7 @@
         <v>10</v>
       </c>
       <c r="V568" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="W568" t="s">
         <v>58</v>
@@ -24862,13 +24841,13 @@
         <v>44378</v>
       </c>
       <c r="J569" t="s">
-        <v>703</v>
-      </c>
-      <c r="L569" t="s">
-        <v>704</v>
-      </c>
-      <c r="M569" s="2">
-        <v>23346</v>
+        <v>700</v>
+      </c>
+      <c r="L569">
+        <v>18</v>
+      </c>
+      <c r="M569">
+        <v>12</v>
       </c>
       <c r="Q569">
         <v>82</v>
@@ -24880,7 +24859,7 @@
         <v>82</v>
       </c>
       <c r="V569" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
       <c r="W569" t="s">
         <v>163</v>
@@ -24921,7 +24900,7 @@
         <v>7</v>
       </c>
       <c r="V570" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
     </row>
     <row r="571" spans="1:24" x14ac:dyDescent="0.2">
@@ -24959,7 +24938,7 @@
         <v>10</v>
       </c>
       <c r="V571" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
     </row>
     <row r="572" spans="1:24" x14ac:dyDescent="0.2">
@@ -24997,7 +24976,7 @@
         <v>7</v>
       </c>
       <c r="V572" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
     </row>
     <row r="573" spans="1:24" x14ac:dyDescent="0.2">
@@ -25035,7 +25014,7 @@
         <v>6</v>
       </c>
       <c r="V573" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
     </row>
     <row r="574" spans="1:24" x14ac:dyDescent="0.2">
@@ -25073,7 +25052,7 @@
         <v>91</v>
       </c>
       <c r="V574" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
     </row>
     <row r="575" spans="1:24" x14ac:dyDescent="0.2">
@@ -25120,7 +25099,7 @@
         <v>82</v>
       </c>
       <c r="V575" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
     </row>
     <row r="576" spans="1:24" x14ac:dyDescent="0.2">
@@ -25152,22 +25131,22 @@
         <v>44428</v>
       </c>
       <c r="P576" t="s">
+        <v>708</v>
+      </c>
+      <c r="R576" t="s">
+        <v>709</v>
+      </c>
+      <c r="S576" t="s">
+        <v>710</v>
+      </c>
+      <c r="V576" t="s">
+        <v>711</v>
+      </c>
+      <c r="W576" t="s">
         <v>712</v>
       </c>
-      <c r="R576" t="s">
+      <c r="X576" t="s">
         <v>713</v>
-      </c>
-      <c r="S576" t="s">
-        <v>714</v>
-      </c>
-      <c r="V576" t="s">
-        <v>715</v>
-      </c>
-      <c r="W576" t="s">
-        <v>716</v>
-      </c>
-      <c r="X576" t="s">
-        <v>717</v>
       </c>
     </row>
     <row r="577" spans="1:24" x14ac:dyDescent="0.2">
@@ -25196,7 +25175,7 @@
         <v>44431</v>
       </c>
       <c r="J577" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="L577">
         <v>0</v>
@@ -25217,7 +25196,7 @@
         <v>77</v>
       </c>
       <c r="V577" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
       <c r="W577" t="s">
         <v>163</v>
@@ -25258,7 +25237,7 @@
         <v>6</v>
       </c>
       <c r="V578" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
     </row>
     <row r="579" spans="1:24" x14ac:dyDescent="0.2">
@@ -25302,7 +25281,7 @@
         <v>100</v>
       </c>
       <c r="V579" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
     </row>
     <row r="580" spans="1:24" x14ac:dyDescent="0.2">
@@ -25343,7 +25322,7 @@
         <v>9</v>
       </c>
       <c r="V580" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
     </row>
     <row r="581" spans="1:24" x14ac:dyDescent="0.2">
@@ -25390,7 +25369,7 @@
         <v>82</v>
       </c>
       <c r="V581" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
     </row>
     <row r="582" spans="1:24" x14ac:dyDescent="0.2">
@@ -25418,11 +25397,11 @@
       <c r="H582" s="1">
         <v>44440</v>
       </c>
-      <c r="L582" s="2">
-        <v>23255</v>
-      </c>
-      <c r="M582" t="s">
-        <v>724</v>
+      <c r="L582">
+        <v>9</v>
+      </c>
+      <c r="M582">
+        <v>14</v>
       </c>
       <c r="Q582">
         <v>96</v>
@@ -25434,10 +25413,10 @@
         <v>92</v>
       </c>
       <c r="V582" t="s">
-        <v>725</v>
+        <v>720</v>
       </c>
       <c r="W582" t="s">
-        <v>726</v>
+        <v>721</v>
       </c>
     </row>
     <row r="583" spans="1:24" x14ac:dyDescent="0.2">
@@ -25462,11 +25441,11 @@
       <c r="H583" s="1">
         <v>44447</v>
       </c>
-      <c r="L583" s="2">
-        <v>23012</v>
-      </c>
-      <c r="M583" t="s">
-        <v>727</v>
+      <c r="L583">
+        <v>1</v>
+      </c>
+      <c r="M583">
+        <v>23</v>
       </c>
       <c r="Q583">
         <v>89</v>
@@ -25478,7 +25457,7 @@
         <v>98</v>
       </c>
       <c r="V583" t="s">
-        <v>728</v>
+        <v>722</v>
       </c>
     </row>
     <row r="584" spans="1:24" x14ac:dyDescent="0.2">
@@ -25525,7 +25504,7 @@
         <v>105</v>
       </c>
       <c r="V584" t="s">
-        <v>729</v>
+        <v>723</v>
       </c>
     </row>
     <row r="585" spans="1:24" x14ac:dyDescent="0.2">
@@ -25569,13 +25548,13 @@
         <v>69</v>
       </c>
       <c r="V585" t="s">
-        <v>730</v>
+        <v>724</v>
       </c>
       <c r="W585" t="s">
         <v>49</v>
       </c>
       <c r="X585" t="s">
-        <v>731</v>
+        <v>725</v>
       </c>
     </row>
     <row r="586" spans="1:24" x14ac:dyDescent="0.2">
@@ -25619,13 +25598,13 @@
         <v>100</v>
       </c>
       <c r="V586" t="s">
-        <v>732</v>
+        <v>726</v>
       </c>
       <c r="W586" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="X586" t="s">
-        <v>733</v>
+        <v>727</v>
       </c>
     </row>
     <row r="587" spans="1:24" x14ac:dyDescent="0.2">
@@ -25666,7 +25645,7 @@
         <v>6</v>
       </c>
       <c r="V587" t="s">
-        <v>734</v>
+        <v>728</v>
       </c>
     </row>
     <row r="588" spans="1:24" x14ac:dyDescent="0.2">
@@ -25710,13 +25689,13 @@
         <v>90</v>
       </c>
       <c r="V588" t="s">
-        <v>735</v>
+        <v>729</v>
       </c>
       <c r="W588" t="s">
         <v>49</v>
       </c>
       <c r="X588" t="s">
-        <v>736</v>
+        <v>730</v>
       </c>
     </row>
     <row r="589" spans="1:24" x14ac:dyDescent="0.2">
@@ -25754,7 +25733,7 @@
         <v>88</v>
       </c>
       <c r="V589" t="s">
-        <v>737</v>
+        <v>731</v>
       </c>
       <c r="W589" t="s">
         <v>163</v>
@@ -25783,7 +25762,7 @@
         <v>44487</v>
       </c>
       <c r="J590" t="s">
-        <v>738</v>
+        <v>732</v>
       </c>
       <c r="P590">
         <v>69</v>
@@ -25798,13 +25777,13 @@
         <v>81</v>
       </c>
       <c r="V590" t="s">
-        <v>739</v>
+        <v>733</v>
       </c>
       <c r="W590" t="s">
         <v>49</v>
       </c>
       <c r="X590" t="s">
-        <v>740</v>
+        <v>734</v>
       </c>
     </row>
     <row r="591" spans="1:24" x14ac:dyDescent="0.2">
@@ -25845,7 +25824,7 @@
         <v>15</v>
       </c>
       <c r="V591" t="s">
-        <v>741</v>
+        <v>735</v>
       </c>
     </row>
     <row r="592" spans="1:24" x14ac:dyDescent="0.2">
@@ -25889,7 +25868,7 @@
         <v>75</v>
       </c>
       <c r="V592" t="s">
-        <v>742</v>
+        <v>736</v>
       </c>
     </row>
     <row r="593" spans="1:26" x14ac:dyDescent="0.2">
@@ -25962,7 +25941,7 @@
         <v>109</v>
       </c>
       <c r="V594" t="s">
-        <v>743</v>
+        <v>737</v>
       </c>
       <c r="W594" t="s">
         <v>58</v>
@@ -26009,7 +25988,7 @@
         <v>100</v>
       </c>
       <c r="V595" t="s">
-        <v>744</v>
+        <v>738</v>
       </c>
     </row>
     <row r="596" spans="1:26" x14ac:dyDescent="0.2">
@@ -26044,7 +26023,7 @@
         <v>6</v>
       </c>
       <c r="V596" t="s">
-        <v>745</v>
+        <v>739</v>
       </c>
     </row>
     <row r="597" spans="1:26" x14ac:dyDescent="0.2">
@@ -26085,13 +26064,13 @@
         <v>7</v>
       </c>
       <c r="V597" t="s">
-        <v>746</v>
+        <v>740</v>
       </c>
       <c r="W597" t="s">
         <v>49</v>
       </c>
       <c r="X597" t="s">
-        <v>747</v>
+        <v>741</v>
       </c>
     </row>
     <row r="598" spans="1:26" x14ac:dyDescent="0.2">
@@ -26158,13 +26137,13 @@
         <v>88</v>
       </c>
       <c r="V599" t="s">
-        <v>748</v>
+        <v>742</v>
       </c>
       <c r="W599" t="s">
         <v>467</v>
       </c>
       <c r="Z599" t="s">
-        <v>749</v>
+        <v>743</v>
       </c>
     </row>
     <row r="600" spans="1:26" x14ac:dyDescent="0.2">
@@ -26205,13 +26184,13 @@
         <v>104</v>
       </c>
       <c r="V600" t="s">
-        <v>750</v>
+        <v>744</v>
       </c>
       <c r="W600" t="s">
         <v>467</v>
       </c>
       <c r="Z600" t="s">
-        <v>751</v>
+        <v>745</v>
       </c>
     </row>
     <row r="601" spans="1:26" x14ac:dyDescent="0.2">
@@ -26252,10 +26231,10 @@
         <v>14</v>
       </c>
       <c r="V601" t="s">
-        <v>752</v>
+        <v>746</v>
       </c>
       <c r="W601" t="s">
-        <v>753</v>
+        <v>747</v>
       </c>
     </row>
   </sheetData>

</xml_diff>